<commit_message>
New value-driven features analysis
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-8.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-8.xlsx
@@ -9,10 +9,6 @@
   <sheets>
     <sheet name="mae" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">mae!$I$4:$I$12</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">mae!$J$4:$J$12</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -71,6 +67,21 @@
   </si>
   <si>
     <t>musartschool</t>
+  </si>
+  <si>
+    <t>Ср. значение</t>
+  </si>
+  <si>
+    <t>Макс</t>
+  </si>
+  <si>
+    <t>Мин</t>
+  </si>
+  <si>
+    <t>Кол-во нулей</t>
+  </si>
+  <si>
+    <t>Анализ признаков в датасете (размер выборки 1897 примеров)</t>
   </si>
 </sst>
 </file>
@@ -1003,16 +1014,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1297,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J57"/>
+  <dimension ref="C3:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,9 +1320,12 @@
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1322,8 +1336,11 @@
       <c r="J3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -1337,8 +1354,23 @@
       <c r="J4" s="3">
         <v>0.28022091714152342</v>
       </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -1354,8 +1386,23 @@
       <c r="J5" s="3">
         <v>0.12950551814581521</v>
       </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" s="4">
+        <v>584.54999999999995</v>
+      </c>
+      <c r="O5" s="4">
+        <v>38482</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -1372,8 +1419,23 @@
       <c r="J6" s="3">
         <v>0.14576179328590291</v>
       </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="4">
+        <v>37.04</v>
+      </c>
+      <c r="O6" s="4">
+        <v>359</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -1390,8 +1452,23 @@
       <c r="J7" s="3">
         <v>3.8414872852975152E-2</v>
       </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="4">
+        <v>44.47</v>
+      </c>
+      <c r="O7" s="4">
+        <v>730</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1408,8 +1485,23 @@
       <c r="J8" s="3">
         <v>1.0340918423375841E-2</v>
       </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O8" s="4">
+        <v>35</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1426,8 +1518,23 @@
       <c r="J9" s="3">
         <v>5.1479099753243752E-2</v>
       </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="O9" s="4">
+        <v>4</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1444,8 +1551,23 @@
       <c r="J10" s="3">
         <v>5.1047374472270618E-2</v>
       </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="O10" s="4">
+        <v>34</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1462,8 +1584,23 @@
       <c r="J11" s="3">
         <v>6.2103540134445211E-2</v>
       </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" s="4">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="O11" s="4">
+        <v>51</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1480,8 +1617,23 @@
       <c r="J12" s="3">
         <v>0.23112596579044811</v>
       </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" s="4">
+        <v>2.91</v>
+      </c>
+      <c r="O12" s="4">
+        <v>53</v>
+      </c>
+      <c r="P12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1492,8 +1644,23 @@
       <c r="E13" s="3">
         <v>107.9239147968667</v>
       </c>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0.86</v>
+      </c>
+      <c r="O13" s="4">
+        <v>8</v>
+      </c>
+      <c r="P13" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1505,7 +1672,7 @@
         <v>94.019204068496549</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1517,7 +1684,7 @@
         <v>107.2600173171996</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>

</xml_diff>

<commit_message>
superdataset-40 vs 41 (MSE)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-8.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-8.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="mae" sheetId="1" r:id="rId1"/>
+    <sheet name="40 vs 41 mse" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -83,6 +84,15 @@
   <si>
     <t>Анализ признаков в датасете (размер выборки 1897 примеров)</t>
   </si>
+  <si>
+    <t>train (MSE)</t>
+  </si>
+  <si>
+    <t>test (MSE)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-40.csv)</t>
+  </si>
 </sst>
 </file>
 
@@ -135,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -145,6 +155,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1311,7 +1324,7 @@
   <dimension ref="C3:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,4 +2196,1197 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:J58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="P51" sqref="P51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1.086960834959154E-3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4.9744983947844698E-3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1.008619893914415E-3</v>
+      </c>
+      <c r="J6" s="5">
+        <v>6.9178327077136937E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f>C6+1</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1.1095543427178691E-3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>5.2350731608704513E-3</v>
+      </c>
+      <c r="H7" s="2">
+        <f>H6+1</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1.0192130743082149E-3</v>
+      </c>
+      <c r="J7" s="5">
+        <v>6.9165606661313484E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:C55" si="0">C7+1</f>
+        <v>3</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1.1812542635738119E-3</v>
+      </c>
+      <c r="E8" s="5">
+        <v>9.8560139207909212E-3</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" ref="H8:H55" si="1">H7+1</f>
+        <v>3</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1.1421940832608221E-3</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1.3617627836967071E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1.1775895924603689E-3</v>
+      </c>
+      <c r="E9" s="5">
+        <v>7.5409129596033467E-3</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1.12174334005007E-3</v>
+      </c>
+      <c r="J9" s="5">
+        <v>2.982431699026321E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.3146362999391201E-3</v>
+      </c>
+      <c r="E10" s="5">
+        <v>7.3206751275493621E-3</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1.1532439325574559E-3</v>
+      </c>
+      <c r="J10" s="5">
+        <v>3.5718031415752798E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.124720934682854E-3</v>
+      </c>
+      <c r="E11" s="5">
+        <v>9.8439719414039634E-3</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1.1236847639598149E-3</v>
+      </c>
+      <c r="J11" s="5">
+        <v>8.1097972015432424E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1.297475059650276E-3</v>
+      </c>
+      <c r="E12" s="5">
+        <v>3.728208713653263E-3</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1.1141373970719971E-3</v>
+      </c>
+      <c r="J12" s="5">
+        <v>6.5635251086878224E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1.1488379721606541E-3</v>
+      </c>
+      <c r="E13" s="5">
+        <v>6.7675776625974824E-3</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I13" s="5">
+        <v>1.0900495601567589E-3</v>
+      </c>
+      <c r="J13" s="5">
+        <v>5.3658013869942829E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1.1544127512620359E-3</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1.2635755346778219E-2</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I14" s="5">
+        <v>1.101335710746776E-3</v>
+      </c>
+      <c r="J14" s="5">
+        <v>7.0417366756601501E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1.093262878974359E-3</v>
+      </c>
+      <c r="E15" s="5">
+        <v>7.968897977640544E-3</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1.1933916534135609E-3</v>
+      </c>
+      <c r="J15" s="5">
+        <v>5.0963349315670666E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1.080037656572603E-3</v>
+      </c>
+      <c r="E16" s="5">
+        <v>9.5933428982676074E-3</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I16" s="5">
+        <v>9.5159696606531333E-4</v>
+      </c>
+      <c r="J16" s="5">
+        <v>8.6978194505271458E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1.3276097805186959E-3</v>
+      </c>
+      <c r="E17" s="5">
+        <v>5.7943396515059151E-3</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I17" s="5">
+        <v>1.0988652015471521E-3</v>
+      </c>
+      <c r="J17" s="5">
+        <v>9.45300616556842E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1.1071591199961E-3</v>
+      </c>
+      <c r="E18" s="5">
+        <v>5.3268386266148949E-3</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I18" s="5">
+        <v>1.1323550059581041E-3</v>
+      </c>
+      <c r="J18" s="5">
+        <v>6.6056229293495602E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D19" s="5">
+        <v>1.3357298684755249E-3</v>
+      </c>
+      <c r="E19" s="5">
+        <v>6.9212712172982867E-3</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I19" s="5">
+        <v>1.2130554405181499E-3</v>
+      </c>
+      <c r="J19" s="5">
+        <v>5.2856855712723532E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1.077621244214323E-3</v>
+      </c>
+      <c r="E20" s="5">
+        <v>8.516041725350287E-3</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I20" s="5">
+        <v>1.0756626567292021E-3</v>
+      </c>
+      <c r="J20" s="5">
+        <v>8.6244757753062857E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1.087902640530053E-3</v>
+      </c>
+      <c r="E21" s="5">
+        <v>7.898775641225101E-3</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1.05298263485322E-3</v>
+      </c>
+      <c r="J21" s="5">
+        <v>5.1352219180681273E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1.259186555707677E-3</v>
+      </c>
+      <c r="E22" s="5">
+        <v>5.0068679171505447E-3</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I22" s="5">
+        <v>1.0792316398785919E-3</v>
+      </c>
+      <c r="J22" s="5">
+        <v>6.4720348466271163E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1.119770139653159E-3</v>
+      </c>
+      <c r="E23" s="5">
+        <v>7.8548425248910411E-3</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I23" s="5">
+        <v>1.0920074331327539E-3</v>
+      </c>
+      <c r="J23" s="5">
+        <v>4.1427929490959192E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1.2605908935769739E-3</v>
+      </c>
+      <c r="E24" s="5">
+        <v>5.9538004326870186E-3</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I24" s="5">
+        <v>1.1618855161627611E-3</v>
+      </c>
+      <c r="J24" s="5">
+        <v>8.0033870754098457E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1.415983026678635E-3</v>
+      </c>
+      <c r="E25" s="5">
+        <v>4.8835185558693791E-3</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I25" s="5">
+        <v>1.1678448362892281E-3</v>
+      </c>
+      <c r="J25" s="5">
+        <v>4.9391580980842264E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1.194158569416326E-3</v>
+      </c>
+      <c r="E26" s="5">
+        <v>8.0930835134021949E-3</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I26" s="5">
+        <v>8.5438253504108142E-4</v>
+      </c>
+      <c r="J26" s="5">
+        <v>1.1416129076116629E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1.240313430959087E-3</v>
+      </c>
+      <c r="E27" s="5">
+        <v>6.483920757942672E-3</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I27" s="5">
+        <v>9.2834272213286953E-4</v>
+      </c>
+      <c r="J27" s="5">
+        <v>6.4782370228056892E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1.1613567556716089E-3</v>
+      </c>
+      <c r="E28" s="5">
+        <v>9.6692271869267855E-3</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I28" s="5">
+        <v>1.053030559981349E-3</v>
+      </c>
+      <c r="J28" s="5">
+        <v>8.0341689051832751E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1.194325485732776E-3</v>
+      </c>
+      <c r="E29" s="5">
+        <v>7.3714355342237156E-3</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I29" s="5">
+        <v>1.0310095904935491E-3</v>
+      </c>
+      <c r="J29" s="5">
+        <v>8.0556143243767954E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1.2891255784088151E-3</v>
+      </c>
+      <c r="E30" s="5">
+        <v>6.479454947865569E-3</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I30" s="5">
+        <v>1.054552415733802E-3</v>
+      </c>
+      <c r="J30" s="5">
+        <v>7.5311513960465426E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1.096953237862405E-3</v>
+      </c>
+      <c r="E31" s="5">
+        <v>6.2979208802106772E-3</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I31" s="5">
+        <v>1.173499981965423E-3</v>
+      </c>
+      <c r="J31" s="5">
+        <v>5.0948812799975424E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1.1053716386686539E-3</v>
+      </c>
+      <c r="E32" s="5">
+        <v>7.96763155703188E-3</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I32" s="5">
+        <v>1.0705747122953841E-3</v>
+      </c>
+      <c r="J32" s="5">
+        <v>6.130147756170443E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D33" s="5">
+        <v>9.9987214233434566E-4</v>
+      </c>
+      <c r="E33" s="5">
+        <v>1.1523594192252389E-2</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I33" s="5">
+        <v>1.137640878225041E-3</v>
+      </c>
+      <c r="J33" s="5">
+        <v>7.5085844056980329E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D34" s="5">
+        <v>1.1579526483260229E-3</v>
+      </c>
+      <c r="E34" s="5">
+        <v>7.992156452975208E-3</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I34" s="5">
+        <v>9.9185175838556548E-4</v>
+      </c>
+      <c r="J34" s="5">
+        <v>7.8707185636483351E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1.2815639011344491E-3</v>
+      </c>
+      <c r="E35" s="5">
+        <v>5.5628092092712429E-3</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I35" s="5">
+        <v>9.8649624172837116E-4</v>
+      </c>
+      <c r="J35" s="5">
+        <v>6.9835319540017711E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D36" s="5">
+        <v>1.098413204671728E-3</v>
+      </c>
+      <c r="E36" s="5">
+        <v>9.2654408184904852E-3</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="I36" s="5">
+        <v>1.101222727037347E-3</v>
+      </c>
+      <c r="J36" s="5">
+        <v>5.6932129980134302E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D37" s="5">
+        <v>1.128733336559972E-3</v>
+      </c>
+      <c r="E37" s="5">
+        <v>4.5769153126197044E-3</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I37" s="5">
+        <v>1.1533354771638229E-3</v>
+      </c>
+      <c r="J37" s="5">
+        <v>6.6323351273186552E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D38" s="5">
+        <v>1.182759254314999E-3</v>
+      </c>
+      <c r="E38" s="5">
+        <v>1.024556569133942E-2</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I38" s="5">
+        <v>1.2445104734854779E-3</v>
+      </c>
+      <c r="J38" s="5">
+        <v>6.8958133653181106E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D39" s="5">
+        <v>1.0250192221662479E-3</v>
+      </c>
+      <c r="E39" s="5">
+        <v>1.624467608039179E-2</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="I39" s="5">
+        <v>1.035101592619781E-3</v>
+      </c>
+      <c r="J39" s="5">
+        <v>4.9246919936179554E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D40" s="5">
+        <v>1.3142155896449001E-3</v>
+      </c>
+      <c r="E40" s="5">
+        <v>5.2214555203015968E-3</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I40" s="5">
+        <v>9.821816673836639E-4</v>
+      </c>
+      <c r="J40" s="5">
+        <v>7.1735938887624159E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D41" s="5">
+        <v>1.0896109340725231E-3</v>
+      </c>
+      <c r="E41" s="5">
+        <v>1.034306978330868E-2</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I41" s="5">
+        <v>1.0927146952327551E-3</v>
+      </c>
+      <c r="J41" s="5">
+        <v>6.5199581249710233E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D42" s="5">
+        <v>1.2251901528042141E-3</v>
+      </c>
+      <c r="E42" s="5">
+        <v>4.4009935339431811E-3</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="I42" s="5">
+        <v>1.242204730927124E-3</v>
+      </c>
+      <c r="J42" s="5">
+        <v>5.6188751481270364E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D43" s="5">
+        <v>1.1634860752699381E-3</v>
+      </c>
+      <c r="E43" s="5">
+        <v>5.4750295069858068E-3</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="I43" s="5">
+        <v>1.031363562627274E-3</v>
+      </c>
+      <c r="J43" s="5">
+        <v>6.4883942585411743E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D44" s="5">
+        <v>1.3259423878643061E-3</v>
+      </c>
+      <c r="E44" s="5">
+        <v>8.0938510117744139E-3</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="I44" s="5">
+        <v>9.3048384908869114E-4</v>
+      </c>
+      <c r="J44" s="5">
+        <v>1.183023757065901E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D45" s="5">
+        <v>9.6457930237897691E-4</v>
+      </c>
+      <c r="E45" s="5">
+        <v>1.219693373912314E-2</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I45" s="5">
+        <v>1.093528412743947E-3</v>
+      </c>
+      <c r="J45" s="5">
+        <v>7.5632652467313207E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D46" s="5">
+        <v>1.158475319765695E-3</v>
+      </c>
+      <c r="E46" s="5">
+        <v>7.8840574652459319E-3</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I46" s="5">
+        <v>1.009805357800025E-3</v>
+      </c>
+      <c r="J46" s="5">
+        <v>8.685120931760916E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D47" s="5">
+        <v>1.114252714894853E-3</v>
+      </c>
+      <c r="E47" s="5">
+        <v>6.3893109574036811E-3</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I47" s="5">
+        <v>1.211805570597023E-3</v>
+      </c>
+      <c r="J47" s="5">
+        <v>6.0801517250706153E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D48" s="5">
+        <v>1.152194167017042E-3</v>
+      </c>
+      <c r="E48" s="5">
+        <v>7.977829764902954E-3</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="I48" s="5">
+        <v>1.1771539768818721E-3</v>
+      </c>
+      <c r="J48" s="5">
+        <v>8.0191834537785851E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D49" s="5">
+        <v>1.30260639310299E-3</v>
+      </c>
+      <c r="E49" s="5">
+        <v>4.6967454916359589E-3</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="I49" s="5">
+        <v>1.1429989349877709E-3</v>
+      </c>
+      <c r="J49" s="5">
+        <v>4.5297200600557946E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D50" s="5">
+        <v>1.286416372071248E-3</v>
+      </c>
+      <c r="E50" s="5">
+        <v>4.6080689072114196E-3</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I50" s="5">
+        <v>1.0927386116294431E-3</v>
+      </c>
+      <c r="J50" s="5">
+        <v>6.0573891948917909E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1.2728082351788879E-3</v>
+      </c>
+      <c r="E51" s="5">
+        <v>6.7864330322855186E-3</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="I51" s="5">
+        <v>1.000371110752578E-3</v>
+      </c>
+      <c r="J51" s="5">
+        <v>9.7455939403653293E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D52" s="5">
+        <v>1.0671163197707059E-3</v>
+      </c>
+      <c r="E52" s="5">
+        <v>8.0892018518708801E-3</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="I52" s="5">
+        <v>1.157351002459867E-3</v>
+      </c>
+      <c r="J52" s="5">
+        <v>4.6179686996546824E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D53" s="5">
+        <v>1.260469419666219E-3</v>
+      </c>
+      <c r="E53" s="5">
+        <v>7.125721521878744E-3</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="I53" s="5">
+        <v>8.8892595684408708E-4</v>
+      </c>
+      <c r="J53" s="5">
+        <v>6.9875669305646078E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D54" s="5">
+        <v>1.243384780777695E-3</v>
+      </c>
+      <c r="E54" s="5">
+        <v>9.3206783947457645E-3</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I54" s="5">
+        <v>1.120570679609032E-3</v>
+      </c>
+      <c r="J54" s="5">
+        <v>6.3107343749248561E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C55" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D55" s="5">
+        <v>1.2135428148311511E-3</v>
+      </c>
+      <c r="E55" s="5">
+        <v>6.3335297024218204E-3</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I55" s="5">
+        <v>1.0857006215636701E-3</v>
+      </c>
+      <c r="J55" s="5">
+        <v>6.8315743031908136E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="5">
+        <f>AVERAGE(D6:D55)</f>
+        <v>1.1814101048328609E-3</v>
+      </c>
+      <c r="E57" s="5">
+        <f>AVERAGE(E6:E55)</f>
+        <v>7.5267593343303074E-3</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I57" s="5">
+        <f>AVERAGE(I6:I55)</f>
+        <v>1.0833710229598409E-3</v>
+      </c>
+      <c r="J57" s="5">
+        <f>AVERAGE(J6:J55)</f>
+        <v>6.9170240431107709E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="5">
+        <f>_xlfn.STDEV.S(D6:D55)</f>
+        <v>9.8608746790317589E-5</v>
+      </c>
+      <c r="E58" s="5">
+        <f>_xlfn.STDEV.S(E6:E55)</f>
+        <v>2.4352373037171437E-3</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I58" s="5">
+        <f>_xlfn.STDEV.S(I6:I55)</f>
+        <v>8.7699277462160711E-5</v>
+      </c>
+      <c r="J58" s="5">
+        <f>_xlfn.STDEV.S(J6:J55)</f>
+        <v>2.0009938178473896E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Features analysis & new plots
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-8.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-8.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="mae" sheetId="1" r:id="rId1"/>
@@ -1321,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:Q57"/>
+  <dimension ref="C2:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,6 +1338,11 @@
     <col min="17" max="17" width="14" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="M2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -1349,8 +1354,20 @@
       <c r="J3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>20</v>
+      <c r="M3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="3:17" x14ac:dyDescent="0.25">
@@ -1367,20 +1384,20 @@
       <c r="J4" s="3">
         <v>0.28022091714152342</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>19</v>
+      <c r="M4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="4">
+        <v>584.54999999999995</v>
+      </c>
+      <c r="O4" s="4">
+        <v>38482</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>904</v>
       </c>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
@@ -1400,19 +1417,19 @@
         <v>0.12950551814581521</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N5" s="4">
-        <v>584.54999999999995</v>
+        <v>37.04</v>
       </c>
       <c r="O5" s="4">
-        <v>38482</v>
+        <v>359</v>
       </c>
       <c r="P5" s="4">
         <v>0</v>
       </c>
       <c r="Q5" s="4">
-        <v>904</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
@@ -1433,19 +1450,19 @@
         <v>0.14576179328590291</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N6" s="4">
-        <v>37.04</v>
+        <v>44.47</v>
       </c>
       <c r="O6" s="4">
-        <v>359</v>
+        <v>730</v>
       </c>
       <c r="P6" s="4">
         <v>0</v>
       </c>
       <c r="Q6" s="4">
-        <v>50</v>
+        <v>786</v>
       </c>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
@@ -1466,19 +1483,19 @@
         <v>3.8414872852975152E-2</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N7" s="4">
-        <v>44.47</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="O7" s="4">
-        <v>730</v>
+        <v>35</v>
       </c>
       <c r="P7" s="4">
         <v>0</v>
       </c>
       <c r="Q7" s="4">
-        <v>786</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
@@ -1499,19 +1516,19 @@
         <v>1.0340918423375841E-2</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N8" s="4">
-        <v>0.56000000000000005</v>
+        <v>0.19</v>
       </c>
       <c r="O8" s="4">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="P8" s="4">
         <v>0</v>
       </c>
       <c r="Q8" s="4">
-        <v>1239</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
@@ -1532,19 +1549,19 @@
         <v>5.1479099753243752E-2</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N9" s="4">
         <v>0.19</v>
       </c>
       <c r="O9" s="4">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="P9" s="4">
         <v>0</v>
       </c>
       <c r="Q9" s="4">
-        <v>1581</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.25">
@@ -1565,19 +1582,19 @@
         <v>5.1047374472270618E-2</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N10" s="4">
-        <v>0.19</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="O10" s="4">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="P10" s="4">
         <v>0</v>
       </c>
       <c r="Q10" s="4">
-        <v>1678</v>
+        <v>980</v>
       </c>
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.25">
@@ -1598,19 +1615,19 @@
         <v>6.2103540134445211E-2</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N11" s="4">
-        <v>2.0299999999999998</v>
+        <v>2.91</v>
       </c>
       <c r="O11" s="4">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P11" s="4">
         <v>0</v>
       </c>
       <c r="Q11" s="4">
-        <v>980</v>
+        <v>537</v>
       </c>
     </row>
     <row r="12" spans="3:17" x14ac:dyDescent="0.25">
@@ -1631,19 +1648,19 @@
         <v>0.23112596579044811</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N12" s="4">
-        <v>2.91</v>
+        <v>0.86</v>
       </c>
       <c r="O12" s="4">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="P12" s="4">
         <v>0</v>
       </c>
       <c r="Q12" s="4">
-        <v>537</v>
+        <v>995</v>
       </c>
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.25">
@@ -1656,21 +1673,6 @@
       </c>
       <c r="E13" s="3">
         <v>107.9239147968667</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0.86</v>
-      </c>
-      <c r="O13" s="4">
-        <v>8</v>
-      </c>
-      <c r="P13" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>995</v>
       </c>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">

</xml_diff>